<commit_message>
Finalização dos casos de teste da funcionalidade 'Gerenciar Usuários'
</commit_message>
<xml_diff>
--- a/Casos de Teste.xlsx
+++ b/Casos de Teste.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victor.guerra\Documents\Dev\qamantis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F5DDEA-D1AC-4D25-A471-A6DFF23B6EF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D77A590A-4179-4590-BAAE-79F46FC65132}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8BD3C4DF-F9CB-4811-9708-DC90EDF83DD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{8BD3C4DF-F9CB-4811-9708-DC90EDF83DD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Gerenciar Usuários" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="147">
   <si>
     <t>Cenário</t>
   </si>
@@ -223,6 +225,322 @@
   </si>
   <si>
     <t>Validar perfis de acesso - administrador</t>
+  </si>
+  <si>
+    <t>Criar conta pela tela de login</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'Criar Conta'</t>
+  </si>
+  <si>
+    <t>1. Usuário 'conta.login' não deve existir na base;
+2. Validação por captcha não deve estar ativada.</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'criar uma nova conta'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a tela 'Criar Conta' com os campos 'Nome de Usuário' e 'E-Mail'.</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'conta.login'</t>
+  </si>
+  <si>
+    <t>Informar o email 'conta.login@tempemailadress.com'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'Registro de conta processado', o nome de usuário e o email informados e grava na base os dados informados pelo usuário.</t>
+  </si>
+  <si>
+    <t>Criar conta pela tela de login com dados inválidos - nome de usuário vazio</t>
+  </si>
+  <si>
+    <t>Informar o email 'conta.login.vazio@tempemailadress.com'</t>
+  </si>
+  <si>
+    <t>1. Validação por captcha não deve estar ativada;
+2. Não deve existir usuário com o email 'conta.login.vazio@tempemailadress.com' na base.</t>
+  </si>
+  <si>
+    <t>O sistema apresenta a mensagem 'O nome de usuário não é válido. Nomes de usuário podem conter apenas letras, números, espaços, hífens, pontos, sinais de mais e sublinhados.'.</t>
+  </si>
+  <si>
+    <t>Criar conta pela tela de login com dados inválidos - nome de usuário inválido</t>
+  </si>
+  <si>
+    <t>1. Validação por captcha não deve estar ativada;
+2. Não deve existir usuário com o email 'conta.login.invalido@tempemailadress.com' na base.</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário '*usuario#125'</t>
+  </si>
+  <si>
+    <t>Informar o email 'conta.login.invalido@tempemailadress.com'</t>
+  </si>
+  <si>
+    <t>Criar conta pela tela de login com dados inválidos - email vazio</t>
+  </si>
+  <si>
+    <t>1. Validação por captcha não deve estar ativada;
+2. Não deve existir usuário com o login 'conta.email.vazio' na base.</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'conta.email.vazio'</t>
+  </si>
+  <si>
+    <t>O sistema apresenta a mensagem 'E-mail inválido.'.</t>
+  </si>
+  <si>
+    <t>1. Validação por captcha não deve estar ativada;
+2. Não deve existir usuário com o login 'conta.email.invalido' na base.</t>
+  </si>
+  <si>
+    <t>Informar o email 'conta.email.invalido.com'</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'conta.email.invalido'</t>
+  </si>
+  <si>
+    <t>Realizar login com o usuário 'admin' e senha 'admin'</t>
+  </si>
+  <si>
+    <t>Acessar o menu 'Gerenciar'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a tela 'Informações do Site'</t>
+  </si>
+  <si>
+    <t>Selecionar aba 'Gerenciar Usuários'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a tela 'Gerenciar Contas'</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'Criar nova conta'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a tela 'Criar nova conta' com os campos:
+1. Nome de usuário;
+2. Nome verdadeiro;
+3. E-Mail;
+4. Nível de acesso;
+5. Habiliado;
+6. Protegido.</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'Criar Usuário'</t>
+  </si>
+  <si>
+    <t>Selecionar o nível de acesso 'relator'</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'criar.conta.relator'</t>
+  </si>
+  <si>
+    <t>Informar o nome verdadeiro 'Conta Relator'</t>
+  </si>
+  <si>
+    <t>Informar o email 'criar.conta.relator@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>Criar conta - relator</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'Usuário criar.conta.relator criado com um nível de acesso de relator'.</t>
+  </si>
+  <si>
+    <t>Criar conta - visualizador</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'criar.conta.visualizador'</t>
+  </si>
+  <si>
+    <t>Informar o nome verdadeiro 'Conta Visualizador'</t>
+  </si>
+  <si>
+    <t>Informar o email 'criar.conta.visualizador@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>Selecionar o nível de acesso 'visualizador'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'Usuário criar.conta.visualizador criado com um nível de acesso de visualizador'.</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'criar.conta.atualizador'</t>
+  </si>
+  <si>
+    <t>Informar o nome verdadeiro 'Conta atualizador'</t>
+  </si>
+  <si>
+    <t>Informar o email 'criar.conta.atualizador@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>Selecionar o nível de acesso 'atualizador'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'Usuário criar.conta.atualizador criado com um nível de acesso de atualizador'.</t>
+  </si>
+  <si>
+    <t>Criar conta - atualizador</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'criar.conta.desenvolvedor'</t>
+  </si>
+  <si>
+    <t>Informar o nome verdadeiro 'Conta desenvolvedor'</t>
+  </si>
+  <si>
+    <t>Informar o email 'criar.conta.desenvolvedor@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>Selecionar o nível de acesso 'desenvolvedor'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'Usuário criar.conta.desenvolvedor criado com um nível de acesso de desenvolvedor'.</t>
+  </si>
+  <si>
+    <t>Criar conta - desenvolvedor</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'criar.conta.gerente'</t>
+  </si>
+  <si>
+    <t>Informar o nome verdadeiro 'Conta gerente'</t>
+  </si>
+  <si>
+    <t>Informar o email 'criar.conta.gerente@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>Selecionar o nível de acesso 'gerente'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'Usuário criar.conta.gerente criado com um nível de acesso de gerente'.</t>
+  </si>
+  <si>
+    <t>Criar conta - gerente</t>
+  </si>
+  <si>
+    <t>Criar conta - administrador</t>
+  </si>
+  <si>
+    <t>Informar o nome de usuário 'criar.conta.administrador'</t>
+  </si>
+  <si>
+    <t>Informar o nome verdadeiro 'Conta administrador'</t>
+  </si>
+  <si>
+    <t>Informar o email 'criar.conta.administrador@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>Selecionar o nível de acesso 'administrador'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'Usuário criar.conta.administrador criado com um nível de acesso de administrador'.</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Não deve existir usuário com login 'criar.conta.visualizador' na base;
+3. Não deve existir usuário com o email 'criar.conta.visualizador@tempemailaddress.com' na base.</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Não deve existir usuário com login 'criar.conta.relator' na base;
+3. Não deve existir usuário com o email 'criar.conta.relator@tempemailaddress.com' na base.</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Não deve existir usuário com login 'criar.conta.atualizador' na base;
+3. Não deve existir usuário com o email 'criar.conta.atualizador@tempemailaddress.com' na base.</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Não deve existir usuário com login 'criar.conta.desenvolvedor' na base;
+3. Não deve existir usuário com o email 'criar.conta.desenvolvedor@tempemailaddress.com' na base.</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Não deve existir usuário com login 'criar.conta.gerente' na base;
+3. Não deve existir usuário com o email 'criar.conta.gerente@tempemailaddress.com' na base.</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Não deve existir usuário com login 'criar.conta.administrador' na base;
+3. Não deve existir usuário com o email 'criar.conta.administrador@tempemailaddress.com' na base.</t>
+  </si>
+  <si>
+    <t>Criar conta com dados inválidos - Nome de usuário vazio</t>
+  </si>
+  <si>
+    <t>Informar o nome verdadeiro 'Conta Usuario Vazio'</t>
+  </si>
+  <si>
+    <t>Informar o email 'criar.conta.usuario.vazio@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>Selecionar o nivel de acesso 'relator'</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador.</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'O nome de usuário não é válido. Nomes de usuário podem conter apenas letras, números, espaços, hífens, pontos, sinais de mais e sublinhados.' e não realiza o cadastro.</t>
+  </si>
+  <si>
+    <t>Informar no campo de pesquisa 'alteracao.conta'</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'Aplicar Filtro'</t>
+  </si>
+  <si>
+    <t>Sistema busca os usuários que possuem o texto informado no nome de usuário, email ou nome real.</t>
+  </si>
+  <si>
+    <t>Clicar no nome de usuário 'alteracao.conta' na tabela de resultados</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a tela 'Alterar Usuário' com os dados do usuário preenchidos.</t>
+  </si>
+  <si>
+    <t>Alterar o nome de usuário para 'conta.alterada'</t>
+  </si>
+  <si>
+    <t>Alterar o email para 'conta.alterada@tempemailaddress.com'</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Usuário 'alteracao.conta' com nível de acesso 'relator' deve existir na base.</t>
+  </si>
+  <si>
+    <t>Alterar o nível de acesso para 'visualizador'</t>
+  </si>
+  <si>
+    <t>Altera o nome verdadeiro para 'Conta Alterada'</t>
+  </si>
+  <si>
+    <t>Clicar no botão 'Alterar Usuário'</t>
+  </si>
+  <si>
+    <t>Sistema altera os dados do usuário e apresenta amensagem 'Operação realizada com sucersso.'.</t>
+  </si>
+  <si>
+    <t>Alterar usuário</t>
+  </si>
+  <si>
+    <t>Alterar usuário com dados inválidos - Nome de usuário vazio</t>
+  </si>
+  <si>
+    <t>1. Usuário 'admin' deve existir com privilégios de administrador;
+2. Usuário 'alteracao.conta.invalido' com nível de acesso 'relator' deve existir na base.</t>
+  </si>
+  <si>
+    <t>Limpar o nome de usuário</t>
+  </si>
+  <si>
+    <t>Alterar o nome de usuário para '*usuario#125'</t>
+  </si>
+  <si>
+    <t>Sistema apresenta a mensagem 'O nome de usuário não é válido. Nomes de usuário podem conter apenas letras, números, espaços, hífens, pontos, sinais de mais e sublinhados.' e não realiza a alteração.</t>
   </si>
 </sst>
 </file>
@@ -254,7 +572,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -433,68 +751,229 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649DAE8C-77D6-439F-9067-7268CF3540DB}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,568 +1304,568 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
+      <c r="A13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2" t="s">
+      <c r="A14" s="22"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="10" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2" t="s">
+      <c r="A20" s="14"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="2" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="10" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="2" t="s">
+      <c r="A24" s="20"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="2" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="2" t="s">
+      <c r="A26" s="20"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="16"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="10" t="s">
+      <c r="A27" s="21"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="2" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2" t="s">
+      <c r="A30" s="17"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="2" t="s">
+      <c r="A31" s="17"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10" t="s">
+      <c r="A32" s="18"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="2" t="s">
+      <c r="A34" s="17"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="2" t="s">
+      <c r="A35" s="17"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="2" t="s">
+      <c r="A36" s="17"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="10" t="s">
+      <c r="A37" s="18"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="2" t="s">
+      <c r="A39" s="17"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="2" t="s">
+      <c r="A40" s="17"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="2" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="10" t="s">
+      <c r="A42" s="18"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="2" t="s">
+      <c r="A44" s="17"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="2" t="s">
+      <c r="A45" s="17"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="2" t="s">
+      <c r="A46" s="17"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="10" t="s">
+      <c r="A47" s="18"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="2" t="s">
+      <c r="A49" s="17"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="2" t="s">
+      <c r="A50" s="17"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="2" t="s">
+      <c r="A51" s="17"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="10" t="s">
+      <c r="A52" s="18"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1418,4 +1897,2070 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7333A022-5203-4E69-834E-B3EB36E2873F}">
+  <dimension ref="A1:D231"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A127" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="25"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="24"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="24"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="24"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="25"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="24"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="24"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="24"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A59" s="24"/>
+      <c r="B59" s="22"/>
+      <c r="C59" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="24"/>
+      <c r="B60" s="22"/>
+      <c r="C60" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="24"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="24"/>
+      <c r="B62" s="22"/>
+      <c r="C62" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="24"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="25"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="24"/>
+      <c r="B66" s="22"/>
+      <c r="C66" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="24"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="24"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A69" s="24"/>
+      <c r="B69" s="22"/>
+      <c r="C69" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="24"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="24"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="24"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="24"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="25"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="24"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="24"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="24"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A79" s="24"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="24"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="24"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A82" s="24"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="24"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="24"/>
+      <c r="B84" s="12"/>
+      <c r="C84" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D84" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C85" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="34"/>
+      <c r="B86" s="22"/>
+      <c r="C86" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="34"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D87" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="34"/>
+      <c r="B88" s="22"/>
+      <c r="C88" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A89" s="34"/>
+      <c r="B89" s="22"/>
+      <c r="C89" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="34"/>
+      <c r="B90" s="22"/>
+      <c r="C90" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
+      <c r="B91" s="22"/>
+      <c r="C91" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="35"/>
+      <c r="B93" s="12"/>
+      <c r="C93" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D93" s="32" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C94" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94" s="39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="34"/>
+      <c r="B95" s="22"/>
+      <c r="C95" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D95" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="34"/>
+      <c r="B96" s="22"/>
+      <c r="C96" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="34"/>
+      <c r="B97" s="22"/>
+      <c r="C97" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A98" s="34"/>
+      <c r="B98" s="22"/>
+      <c r="C98" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D98" s="41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="34"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D99" s="41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="34"/>
+      <c r="B100" s="22"/>
+      <c r="C100" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="34"/>
+      <c r="B101" s="22"/>
+      <c r="C101" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D101" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="34"/>
+      <c r="B102" s="22"/>
+      <c r="C102" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D102" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="34"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D103" s="37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C104" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" s="40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="34"/>
+      <c r="B105" s="22"/>
+      <c r="C105" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="34"/>
+      <c r="B106" s="22"/>
+      <c r="C106" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="34"/>
+      <c r="B107" s="22"/>
+      <c r="C107" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="34"/>
+      <c r="B108" s="22"/>
+      <c r="C108" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D108" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="34"/>
+      <c r="B109" s="22"/>
+      <c r="C109" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D109" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="34"/>
+      <c r="B110" s="22"/>
+      <c r="C110" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="34"/>
+      <c r="B111" s="22"/>
+      <c r="C111" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D111" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="34"/>
+      <c r="B112" s="22"/>
+      <c r="C112" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D112" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="34"/>
+      <c r="B113" s="22"/>
+      <c r="C113" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="34"/>
+      <c r="B114" s="22"/>
+      <c r="C114" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="35"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C116" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D116" s="40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="24"/>
+      <c r="B117" s="22"/>
+      <c r="C117" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D117" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="24"/>
+      <c r="B118" s="22"/>
+      <c r="C118" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D118" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="24"/>
+      <c r="B119" s="22"/>
+      <c r="C119" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D119" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="24"/>
+      <c r="B120" s="22"/>
+      <c r="C120" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D120" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="24"/>
+      <c r="B121" s="22"/>
+      <c r="C121" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D121" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A122" s="24"/>
+      <c r="B122" s="22"/>
+      <c r="C122" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D122" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="24"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D123" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="24"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D124" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="24"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D125" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="24"/>
+      <c r="B126" s="22"/>
+      <c r="C126" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D126" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="25"/>
+      <c r="B127" s="12"/>
+      <c r="C127" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D127" s="37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C128" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D128" s="40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="24"/>
+      <c r="B129" s="22"/>
+      <c r="C129" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D129" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="24"/>
+      <c r="B130" s="22"/>
+      <c r="C130" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D130" s="30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="24"/>
+      <c r="B131" s="22"/>
+      <c r="C131" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D131" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A132" s="24"/>
+      <c r="B132" s="22"/>
+      <c r="C132" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D132" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="24"/>
+      <c r="B133" s="22"/>
+      <c r="C133" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D133" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="24"/>
+      <c r="B134" s="22"/>
+      <c r="C134" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D134" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="24"/>
+      <c r="B135" s="22"/>
+      <c r="C135" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D135" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="24"/>
+      <c r="B136" s="22"/>
+      <c r="C136" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D136" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A137" s="24"/>
+      <c r="B137" s="22"/>
+      <c r="C137" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D137" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="24"/>
+      <c r="B138" s="22"/>
+      <c r="C138" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D138" s="30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="25"/>
+      <c r="B139" s="12"/>
+      <c r="C139" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D139" s="37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="38"/>
+      <c r="B140" s="1"/>
+      <c r="C140" s="28"/>
+      <c r="D140" s="28"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="38"/>
+      <c r="B141" s="1"/>
+      <c r="C141" s="28"/>
+      <c r="D141" s="28"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="38"/>
+      <c r="B142" s="1"/>
+      <c r="C142" s="28"/>
+      <c r="D142" s="28"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="38"/>
+      <c r="B143" s="1"/>
+      <c r="C143" s="28"/>
+      <c r="D143" s="28"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="38"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="28"/>
+      <c r="D144" s="28"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="38"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="28"/>
+      <c r="D145" s="28"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="38"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="28"/>
+      <c r="D146" s="28"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="38"/>
+      <c r="B147" s="1"/>
+      <c r="C147" s="28"/>
+      <c r="D147" s="28"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="38"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="28"/>
+      <c r="D148" s="28"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="38"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="28"/>
+      <c r="D149" s="28"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="38"/>
+      <c r="B150" s="1"/>
+      <c r="C150" s="28"/>
+      <c r="D150" s="28"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="38"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="28"/>
+      <c r="D151" s="28"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="38"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="28"/>
+      <c r="D152" s="28"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="38"/>
+      <c r="B153" s="1"/>
+      <c r="C153" s="28"/>
+      <c r="D153" s="28"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="38"/>
+      <c r="B154" s="1"/>
+      <c r="C154" s="28"/>
+      <c r="D154" s="28"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="38"/>
+      <c r="B155" s="1"/>
+      <c r="C155" s="28"/>
+      <c r="D155" s="28"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="38"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="28"/>
+      <c r="D156" s="28"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="38"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="28"/>
+      <c r="D157" s="28"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="38"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="28"/>
+      <c r="D158" s="28"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="38"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="28"/>
+      <c r="D159" s="28"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="38"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="28"/>
+      <c r="D160" s="28"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="38"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="28"/>
+      <c r="D161" s="28"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="38"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="28"/>
+      <c r="D162" s="28"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="38"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="28"/>
+      <c r="D163" s="28"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="38"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="28"/>
+      <c r="D164" s="28"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="38"/>
+      <c r="B165" s="1"/>
+      <c r="C165" s="28"/>
+      <c r="D165" s="28"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="38"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="28"/>
+      <c r="D166" s="28"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="38"/>
+      <c r="B167" s="1"/>
+      <c r="C167" s="28"/>
+      <c r="D167" s="28"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="38"/>
+      <c r="B168" s="1"/>
+      <c r="C168" s="28"/>
+      <c r="D168" s="28"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="38"/>
+      <c r="B169" s="1"/>
+      <c r="C169" s="28"/>
+      <c r="D169" s="28"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="38"/>
+      <c r="B170" s="1"/>
+      <c r="C170" s="28"/>
+      <c r="D170" s="28"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="38"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="28"/>
+      <c r="D171" s="28"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="38"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="28"/>
+      <c r="D172" s="28"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="38"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="28"/>
+      <c r="D173" s="28"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="38"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="28"/>
+      <c r="D174" s="28"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="38"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="28"/>
+      <c r="D175" s="28"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="38"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="28"/>
+      <c r="D176" s="28"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="38"/>
+      <c r="B177" s="1"/>
+      <c r="C177" s="28"/>
+      <c r="D177" s="28"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="38"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="28"/>
+      <c r="D178" s="28"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="38"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="28"/>
+      <c r="D179" s="28"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="38"/>
+      <c r="B180" s="1"/>
+      <c r="C180" s="28"/>
+      <c r="D180" s="28"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="38"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="28"/>
+      <c r="D181" s="28"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="38"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="28"/>
+      <c r="D182" s="28"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="38"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="28"/>
+      <c r="D183" s="28"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="38"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="28"/>
+      <c r="D184" s="28"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="38"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="28"/>
+      <c r="D185" s="28"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="38"/>
+      <c r="B186" s="1"/>
+      <c r="C186" s="28"/>
+      <c r="D186" s="28"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="38"/>
+      <c r="B187" s="1"/>
+      <c r="C187" s="28"/>
+      <c r="D187" s="28"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="38"/>
+      <c r="B188" s="1"/>
+      <c r="C188" s="28"/>
+      <c r="D188" s="28"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="38"/>
+      <c r="B189" s="1"/>
+      <c r="C189" s="28"/>
+      <c r="D189" s="28"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="38"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="28"/>
+      <c r="D190" s="28"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="38"/>
+      <c r="B191" s="1"/>
+      <c r="C191" s="28"/>
+      <c r="D191" s="28"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="38"/>
+      <c r="B192" s="1"/>
+      <c r="C192" s="28"/>
+      <c r="D192" s="28"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="38"/>
+      <c r="B193" s="1"/>
+      <c r="C193" s="28"/>
+      <c r="D193" s="28"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="38"/>
+      <c r="B194" s="1"/>
+      <c r="C194" s="28"/>
+      <c r="D194" s="28"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="38"/>
+      <c r="B195" s="1"/>
+      <c r="C195" s="28"/>
+      <c r="D195" s="28"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="38"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="28"/>
+      <c r="D196" s="28"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="38"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="28"/>
+      <c r="D197" s="28"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="38"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="28"/>
+      <c r="D198" s="28"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="38"/>
+      <c r="B199" s="1"/>
+      <c r="C199" s="28"/>
+      <c r="D199" s="28"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="38"/>
+      <c r="B200" s="1"/>
+      <c r="C200" s="28"/>
+      <c r="D200" s="28"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="38"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="28"/>
+      <c r="D201" s="28"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="38"/>
+      <c r="B202" s="1"/>
+      <c r="C202" s="28"/>
+      <c r="D202" s="28"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="38"/>
+      <c r="B203" s="1"/>
+      <c r="C203" s="28"/>
+      <c r="D203" s="28"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="38"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="28"/>
+      <c r="D204" s="28"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="38"/>
+      <c r="B205" s="1"/>
+      <c r="C205" s="28"/>
+      <c r="D205" s="28"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="38"/>
+      <c r="B206" s="1"/>
+      <c r="C206" s="28"/>
+      <c r="D206" s="28"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="38"/>
+      <c r="B207" s="1"/>
+      <c r="C207" s="28"/>
+      <c r="D207" s="28"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="38"/>
+      <c r="B208" s="1"/>
+      <c r="C208" s="28"/>
+      <c r="D208" s="28"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="38"/>
+      <c r="B209" s="1"/>
+      <c r="C209" s="28"/>
+      <c r="D209" s="28"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="38"/>
+      <c r="B210" s="1"/>
+      <c r="C210" s="28"/>
+      <c r="D210" s="28"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="38"/>
+      <c r="B211" s="1"/>
+      <c r="C211" s="28"/>
+      <c r="D211" s="28"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="38"/>
+      <c r="B212" s="1"/>
+      <c r="C212" s="28"/>
+      <c r="D212" s="28"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="38"/>
+      <c r="B213" s="1"/>
+      <c r="C213" s="28"/>
+      <c r="D213" s="28"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="38"/>
+      <c r="B214" s="1"/>
+      <c r="C214" s="28"/>
+      <c r="D214" s="28"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="38"/>
+      <c r="B215" s="1"/>
+      <c r="C215" s="28"/>
+      <c r="D215" s="28"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="38"/>
+      <c r="B216" s="1"/>
+      <c r="C216" s="28"/>
+      <c r="D216" s="28"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="38"/>
+      <c r="B217" s="1"/>
+      <c r="C217" s="28"/>
+      <c r="D217" s="28"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="38"/>
+      <c r="B218" s="1"/>
+      <c r="C218" s="28"/>
+      <c r="D218" s="28"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="38"/>
+      <c r="B219" s="1"/>
+      <c r="C219" s="28"/>
+      <c r="D219" s="28"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="38"/>
+      <c r="B220" s="1"/>
+      <c r="C220" s="28"/>
+      <c r="D220" s="28"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="38"/>
+      <c r="B221" s="1"/>
+      <c r="C221" s="28"/>
+      <c r="D221" s="28"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="38"/>
+      <c r="B222" s="1"/>
+      <c r="C222" s="28"/>
+      <c r="D222" s="28"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="38"/>
+      <c r="B223" s="1"/>
+      <c r="C223" s="28"/>
+      <c r="D223" s="28"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="38"/>
+      <c r="B224" s="1"/>
+      <c r="C224" s="28"/>
+      <c r="D224" s="28"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="38"/>
+      <c r="B225" s="1"/>
+      <c r="C225" s="28"/>
+      <c r="D225" s="28"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="38"/>
+      <c r="B226" s="1"/>
+      <c r="C226" s="28"/>
+      <c r="D226" s="28"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="38"/>
+      <c r="B227" s="1"/>
+      <c r="C227" s="28"/>
+      <c r="D227" s="28"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="38"/>
+      <c r="B228" s="1"/>
+      <c r="C228" s="28"/>
+      <c r="D228" s="28"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="38"/>
+      <c r="B229" s="1"/>
+      <c r="C229" s="28"/>
+      <c r="D229" s="28"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="38"/>
+      <c r="B230" s="1"/>
+      <c r="C230" s="28"/>
+      <c r="D230" s="28"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="38"/>
+      <c r="B231" s="1"/>
+      <c r="C231" s="28"/>
+      <c r="D231" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="B116:B127"/>
+    <mergeCell ref="A116:A127"/>
+    <mergeCell ref="A128:A139"/>
+    <mergeCell ref="B128:B139"/>
+    <mergeCell ref="B85:B93"/>
+    <mergeCell ref="A85:A93"/>
+    <mergeCell ref="A94:A103"/>
+    <mergeCell ref="B94:B103"/>
+    <mergeCell ref="B104:B115"/>
+    <mergeCell ref="A104:A115"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="A65:A74"/>
+    <mergeCell ref="B65:B74"/>
+    <mergeCell ref="A75:A84"/>
+    <mergeCell ref="B75:B84"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="B35:B44"/>
+    <mergeCell ref="A45:A54"/>
+    <mergeCell ref="B45:B54"/>
+    <mergeCell ref="A55:A64"/>
+    <mergeCell ref="B55:B64"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>